<commit_message>
ka cs trent 3-7
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-trend-3.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-trend-3.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -723,11 +723,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85927040"/>
-        <c:axId val="85928576"/>
+        <c:axId val="86779008"/>
+        <c:axId val="86780544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85927040"/>
+        <c:axId val="86779008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -736,14 +736,14 @@
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85928576"/>
+        <c:crossAx val="86780544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85928576"/>
+        <c:axId val="86780544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +752,7 @@
         <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85927040"/>
+        <c:crossAx val="86779008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -770,7 +770,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001277" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001277" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1345,9 +1345,7 @@
       <c r="C15" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="D15" s="11"/>
       <c r="E15" s="14"/>
       <c r="F15" s="23"/>
       <c r="G15" s="6"/>

</xml_diff>